<commit_message>
Improvements to Load and Merge functions.
</commit_message>
<xml_diff>
--- a/CANConfig.xlsx
+++ b/CANConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\EclipsePython\PythonWorkspace\CANDB_py\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BB2065-E6B6-478A-86FC-DB4707988021}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B8727-C0FB-4C58-AB45-947645557808}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22815" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>